<commit_message>
feat: Add Excel Controller - instance add_data_to_excel
</commit_message>
<xml_diff>
--- a/money_control.xlsx
+++ b/money_control.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,32 +437,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ingresos</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Gastos</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Fecha</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>750</v>
+          <t>Ingresos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gastos</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2020-09-05</t>
+          <t>Fecha</t>
         </is>
       </c>
     </row>
@@ -470,27 +465,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2020-09-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B5" t="n">
         <v>60</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2020-09-07</t>
-        </is>
+      <c r="C4" s="1" t="n">
+        <v>44083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: bug whit type_of_data funtion in main.py
</commit_message>
<xml_diff>
--- a/money_control.xlsx
+++ b/money_control.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -461,14 +458,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>44083</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2020-09-07</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Starting to develop the excel edition - excel_controller.py - add_data_to_excel instance
</commit_message>
<xml_diff>
--- a/money_control.xlsx
+++ b/money_control.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Control de Gastos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,66 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Saldo inicial:</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ingresos</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Gastos</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2020-09-07</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testing the Telegram API bot
</commit_message>
<xml_diff>
--- a/money_control.xlsx
+++ b/money_control.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Control de Gastos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +416,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Saldo inicial:</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ingresos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gastos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>44087</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>